<commit_message>
update user manual with new genetics
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/ParameterFile.xlsx
+++ b/doc/Manual/Batchmode/ParameterFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter2\doc\Manual\Batchmode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\Desktop\RS3_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF33D48-5E11-43C3-A873-624EEE186DCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED558CA-9133-425F-96CC-9ECD42827A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="116">
   <si>
     <t>Replicates</t>
   </si>
@@ -450,9 +450,6 @@
     <t>Output start year for individuals file</t>
   </si>
   <si>
-    <t>Output start year for genetics file</t>
-  </si>
-  <si>
     <t>OutStartTraitCell</t>
   </si>
   <si>
@@ -495,12 +492,6 @@
     <t>Output interval for individuals file</t>
   </si>
   <si>
-    <t>OutIntGenetic</t>
-  </si>
-  <si>
-    <t>Output interval for genetics file</t>
-  </si>
-  <si>
     <t>OutIntTraitCell</t>
   </si>
   <si>
@@ -519,28 +510,13 @@
     <t>Output interval for connectivity matrix</t>
   </si>
   <si>
-    <t>OutStartGenetic</t>
-  </si>
-  <si>
     <t>Local extinction probability at optimum (if gradient = 3, otherwise 0)</t>
   </si>
   <si>
-    <t>OutGenCrossTab</t>
-  </si>
-  <si>
-    <t>Output genetics as a cross table: 0 = no, 1 = yes</t>
-  </si>
-  <si>
     <t>Absorbing</t>
   </si>
   <si>
     <t>Landscape boundary and any 'no-data' areas are absorbing: 0 = No, 1 = Yes</t>
-  </si>
-  <si>
-    <t>OutGenType</t>
-  </si>
-  <si>
-    <t>Output genetics for: 0 = juveniles only, 1 =  all individuals, 2 = adults only</t>
   </si>
   <si>
     <t>Proportion of males at birth in a sexual population (actually the probability that an individual is male; hence a skewed sex-ratio can arise in a small population)</t>
@@ -654,6 +630,12 @@
   </si>
   <si>
     <t>Must be 0 for an artificial landscape or if there is only 1 replicate</t>
+  </si>
+  <si>
+    <t>FixReplicateSeed</t>
+  </si>
+  <si>
+    <t>Use the same seed for all replicates. 0 = No, 1 = Yes</t>
   </si>
 </sst>
 </file>
@@ -1298,21 +1280,20 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46"/>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" xfId="46" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1321,10 +1302,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1336,7 +1314,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1363,10 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
@@ -1375,28 +1350,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="46" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1469,9 +1432,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1509,9 +1472,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1544,26 +1507,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1596,26 +1542,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1789,773 +1718,653 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="25" customWidth="1"/>
-    <col min="4" max="4" width="58.5703125" style="25" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="11"/>
+    <col min="1" max="1" width="18.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="58.5546875" style="22" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="D30" s="30"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="35"/>
-    </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="C31" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="28"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="C32" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="28"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="C33" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="28"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="28"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="28"/>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="C45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="C46" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="D30" s="37"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="35"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" s="35"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="35"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="35"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="35"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="D40" s="35"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="35"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="B42" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="35"/>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" s="35"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="D44" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="B46" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="24"/>
-    </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="24"/>
-    </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C53" s="24"/>
-    </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="24"/>
-    </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C55" s="24"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="24"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="24"/>
-    </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="24"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="24"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="24"/>
-    </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="24"/>
-    </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C62" s="24"/>
-    </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="24"/>
-    </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C64" s="24"/>
-    </row>
-    <row r="65" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="24"/>
-    </row>
-    <row r="66" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C66" s="24"/>
-    </row>
-    <row r="67" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="24"/>
-    </row>
-    <row r="68" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C68" s="24"/>
-    </row>
-    <row r="69" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="24"/>
-    </row>
-    <row r="70" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="24"/>
-    </row>
-    <row r="71" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C71" s="24"/>
-    </row>
-    <row r="72" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C72" s="24"/>
-    </row>
-    <row r="73" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="24"/>
-    </row>
-    <row r="74" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="24"/>
-    </row>
-    <row r="75" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="24"/>
-    </row>
-    <row r="76" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C76" s="24"/>
-    </row>
-    <row r="77" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C77" s="24"/>
-    </row>
-    <row r="78" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C78" s="24"/>
+      <c r="D47" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2568,218 +2377,205 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AX8"/>
+  <dimension ref="A1:AU8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="AU1" sqref="AU1:AU1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.5703125" style="1" customWidth="1"/>
-    <col min="50" max="50" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="16384" width="9.140625" style="1"/>
+    <col min="31" max="31" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.5546875" style="1" customWidth="1"/>
+    <col min="46" max="46" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="28" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:47" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="28" t="s">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="R1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="S1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="T1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="U1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="V1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="W1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="X1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="29" t="s">
+      <c r="Z1" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="30" t="s">
+      <c r="AB1" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="AC1" s="30" t="s">
+      <c r="AC1" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="AD1" s="30" t="s">
+      <c r="AD1" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="AE1" s="31" t="s">
+      <c r="AE1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" s="31" t="s">
+      <c r="AF1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AG1" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH1" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI1" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ1" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK1" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL1" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="AM1" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="AN1" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="AO1" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AP1" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="AQ1" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="AR1" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="AS1" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="AT1" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU1" s="31" t="s">
+      <c r="AG1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AV1" s="31" t="s">
+      <c r="AR1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AW1" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="AX1" s="31" t="s">
+      <c r="AS1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AT1" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="AU1" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -2886,10 +2682,10 @@
         <v>0</v>
       </c>
       <c r="AJ2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL2" s="1">
         <v>0</v>
@@ -2903,13 +2699,13 @@
       <c r="AO2" s="1">
         <v>0</v>
       </c>
-      <c r="AP2" s="1">
+      <c r="AP2" s="2">
         <v>0</v>
       </c>
       <c r="AQ2" s="1">
         <v>0</v>
       </c>
-      <c r="AR2" s="1">
+      <c r="AR2" s="2">
         <v>0</v>
       </c>
       <c r="AS2" s="1">
@@ -2921,17 +2717,8 @@
       <c r="AU2" s="1">
         <v>0</v>
       </c>
-      <c r="AV2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -3038,52 +2825,43 @@
         <v>0</v>
       </c>
       <c r="AJ3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL3" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM3" s="1">
+        <v>10</v>
+      </c>
+      <c r="AN3" s="1">
         <v>5</v>
       </c>
-      <c r="AN3" s="1">
-        <v>10</v>
-      </c>
       <c r="AO3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AP3" s="1">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>1</v>
       </c>
       <c r="AQ3" s="1">
         <v>1</v>
       </c>
       <c r="AR3" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AS3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AT3" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AT3" s="1">
+        <v>0</v>
       </c>
       <c r="AU3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AW3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -3190,16 +2968,16 @@
         <v>0</v>
       </c>
       <c r="AJ4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM4" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AN4" s="1">
         <v>0</v>
@@ -3207,14 +2985,14 @@
       <c r="AO4" s="1">
         <v>0</v>
       </c>
-      <c r="AP4" s="1">
-        <v>0</v>
+      <c r="AP4" s="2">
+        <v>2</v>
       </c>
       <c r="AQ4" s="1">
         <v>0</v>
       </c>
-      <c r="AR4" s="1">
-        <v>0</v>
+      <c r="AR4" s="2">
+        <v>2</v>
       </c>
       <c r="AS4" s="1">
         <v>0</v>
@@ -3225,17 +3003,8 @@
       <c r="AU4" s="1">
         <v>0</v>
       </c>
-      <c r="AV4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AW4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -3342,16 +3111,16 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL5" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AM5" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AN5" s="1">
         <v>0</v>
@@ -3359,14 +3128,14 @@
       <c r="AO5" s="1">
         <v>0</v>
       </c>
-      <c r="AP5" s="1">
-        <v>0</v>
+      <c r="AP5" s="2">
+        <v>-1</v>
       </c>
       <c r="AQ5" s="1">
         <v>0</v>
       </c>
-      <c r="AR5" s="1">
-        <v>0</v>
+      <c r="AR5" s="2">
+        <v>-1</v>
       </c>
       <c r="AS5" s="1">
         <v>0</v>
@@ -3377,17 +3146,8 @@
       <c r="AU5" s="1">
         <v>0</v>
       </c>
-      <c r="AV5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AW5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -3494,13 +3254,13 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="1">
         <v>1</v>
       </c>
       <c r="AL6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM6" s="1">
         <v>0</v>
@@ -3512,34 +3272,25 @@
         <v>0</v>
       </c>
       <c r="AP6" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AQ6" s="1">
         <v>0</v>
       </c>
-      <c r="AR6" s="1">
-        <v>0</v>
+      <c r="AR6" s="2">
+        <v>1</v>
       </c>
       <c r="AS6" s="1">
         <v>0</v>
       </c>
-      <c r="AT6" s="1">
-        <v>10</v>
+      <c r="AT6" s="2">
+        <v>1</v>
       </c>
       <c r="AU6" s="1">
         <v>0</v>
       </c>
-      <c r="AV6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AW6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -3646,13 +3397,13 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7" s="1">
         <v>1</v>
       </c>
       <c r="AL7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM7" s="1">
         <v>0</v>
@@ -3664,13 +3415,13 @@
         <v>0</v>
       </c>
       <c r="AP7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AS7" s="1">
         <v>0</v>
@@ -3679,19 +3430,10 @@
         <v>1</v>
       </c>
       <c r="AU7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV7" s="1">
-        <v>10</v>
-      </c>
-      <c r="AW7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -3798,13 +3540,13 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="1">
         <v>1</v>
       </c>
       <c r="AL8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM8" s="1">
         <v>0</v>
@@ -3816,30 +3558,21 @@
         <v>0</v>
       </c>
       <c r="AP8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS8" s="1">
         <v>0</v>
       </c>
       <c r="AT8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AU8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV8" s="1">
-        <v>2</v>
-      </c>
-      <c r="AW8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3851,66 +3584,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AV8"/>
+  <dimension ref="A1:AS8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.5703125" style="1" customWidth="1"/>
-    <col min="48" max="48" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="9.140625" style="1"/>
+    <col min="29" max="29" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5546875" style="1" customWidth="1"/>
+    <col min="44" max="44" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -3920,8 +3649,8 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>111</v>
+      <c r="D1" s="23" t="s">
+        <v>105</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -3986,77 +3715,68 @@
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="Z1" s="23" t="s">
         <v>72</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="AC1" s="31" t="s">
+      <c r="AC1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="31" t="s">
+      <c r="AD1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF1" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG1" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH1" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="AI1" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ1" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK1" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL1" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM1" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AN1" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="AO1" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="AP1" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="AQ1" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="AR1" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS1" s="31" t="s">
+      <c r="AE1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AT1" s="31" t="s">
+      <c r="AP1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AU1" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="AV1" s="31" t="s">
+      <c r="AQ1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AR1" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AS1" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -4157,10 +3877,10 @@
         <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2" s="1">
         <v>0</v>
@@ -4174,13 +3894,13 @@
       <c r="AM2" s="1">
         <v>0</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AN2" s="2">
         <v>0</v>
       </c>
       <c r="AO2" s="1">
         <v>0</v>
       </c>
-      <c r="AP2" s="1">
+      <c r="AP2" s="2">
         <v>0</v>
       </c>
       <c r="AQ2" s="1">
@@ -4192,17 +3912,8 @@
       <c r="AS2" s="1">
         <v>0</v>
       </c>
-      <c r="AT2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -4303,52 +4014,43 @@
         <v>0</v>
       </c>
       <c r="AH3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK3" s="1">
+        <v>10</v>
+      </c>
+      <c r="AL3" s="1">
         <v>5</v>
       </c>
-      <c r="AL3" s="1">
-        <v>10</v>
-      </c>
       <c r="AM3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>1</v>
       </c>
       <c r="AO3" s="1">
         <v>1</v>
       </c>
       <c r="AP3" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AQ3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AR3" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>0</v>
       </c>
       <c r="AS3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AU3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -4449,16 +4151,16 @@
         <v>0</v>
       </c>
       <c r="AH4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK4" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="1">
         <v>0</v>
@@ -4466,14 +4168,14 @@
       <c r="AM4" s="1">
         <v>0</v>
       </c>
-      <c r="AN4" s="1">
-        <v>0</v>
+      <c r="AN4" s="2">
+        <v>2</v>
       </c>
       <c r="AO4" s="1">
         <v>0</v>
       </c>
-      <c r="AP4" s="1">
-        <v>0</v>
+      <c r="AP4" s="2">
+        <v>2</v>
       </c>
       <c r="AQ4" s="1">
         <v>0</v>
@@ -4484,17 +4186,8 @@
       <c r="AS4" s="1">
         <v>0</v>
       </c>
-      <c r="AT4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AU4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -4546,10 +4239,10 @@
       <c r="Q5" s="1">
         <v>88</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="1">
         <v>1.6</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="1">
         <v>2.1</v>
       </c>
       <c r="T5" s="2">
@@ -4595,16 +4288,16 @@
         <v>0</v>
       </c>
       <c r="AH5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK5" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AL5" s="1">
         <v>0</v>
@@ -4612,14 +4305,14 @@
       <c r="AM5" s="1">
         <v>0</v>
       </c>
-      <c r="AN5" s="1">
-        <v>0</v>
+      <c r="AN5" s="2">
+        <v>-1</v>
       </c>
       <c r="AO5" s="1">
         <v>0</v>
       </c>
-      <c r="AP5" s="1">
-        <v>0</v>
+      <c r="AP5" s="2">
+        <v>-1</v>
       </c>
       <c r="AQ5" s="1">
         <v>0</v>
@@ -4630,17 +4323,8 @@
       <c r="AS5" s="1">
         <v>0</v>
       </c>
-      <c r="AT5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AU5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV5" s="2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -4692,10 +4376,10 @@
       <c r="Q6" s="1">
         <v>0.5</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="1">
         <v>1.4</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="1">
         <v>2.9</v>
       </c>
       <c r="T6" s="2">
@@ -4741,13 +4425,13 @@
         <v>0</v>
       </c>
       <c r="AH6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" s="1">
         <v>1</v>
       </c>
       <c r="AJ6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="1">
         <v>0</v>
@@ -4759,34 +4443,25 @@
         <v>0</v>
       </c>
       <c r="AN6" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO6" s="1">
         <v>0</v>
       </c>
-      <c r="AP6" s="1">
-        <v>0</v>
+      <c r="AP6" s="2">
+        <v>1</v>
       </c>
       <c r="AQ6" s="1">
         <v>0</v>
       </c>
-      <c r="AR6" s="1">
-        <v>10</v>
+      <c r="AR6" s="2">
+        <v>1</v>
       </c>
       <c r="AS6" s="1">
         <v>0</v>
       </c>
-      <c r="AT6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -4838,10 +4513,10 @@
       <c r="Q7" s="1">
         <v>88</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="1">
         <v>2</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="1">
         <v>3</v>
       </c>
       <c r="T7" s="2">
@@ -4887,13 +4562,13 @@
         <v>0</v>
       </c>
       <c r="AH7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7" s="1">
         <v>1</v>
       </c>
       <c r="AJ7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="1">
         <v>0</v>
@@ -4905,13 +4580,13 @@
         <v>0</v>
       </c>
       <c r="AN7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AQ7" s="1">
         <v>0</v>
@@ -4920,19 +4595,10 @@
         <v>1</v>
       </c>
       <c r="AS7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT7" s="1">
-        <v>10</v>
-      </c>
-      <c r="AU7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -4984,10 +4650,10 @@
       <c r="Q8" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="1">
         <v>1.552</v>
       </c>
-      <c r="S8" s="4">
+      <c r="S8" s="1">
         <v>1.5569999999999999</v>
       </c>
       <c r="T8" s="2">
@@ -5033,13 +4699,13 @@
         <v>0</v>
       </c>
       <c r="AH8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8" s="1">
         <v>1</v>
       </c>
       <c r="AJ8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="1">
         <v>0</v>
@@ -5051,30 +4717,21 @@
         <v>0</v>
       </c>
       <c r="AN8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ8" s="1">
         <v>0</v>
       </c>
       <c r="AR8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT8" s="1">
-        <v>2</v>
-      </c>
-      <c r="AU8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="1">
         <v>0</v>
       </c>
     </row>
@@ -5085,65 +4742,61 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AV8"/>
+  <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="AS9" sqref="AS9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.5703125" style="1" customWidth="1"/>
-    <col min="48" max="48" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="16384" width="9.140625" style="1"/>
+    <col min="29" max="29" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5546875" style="1" customWidth="1"/>
+    <col min="44" max="44" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -5153,8 +4806,8 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>111</v>
+      <c r="D1" s="23" t="s">
+        <v>105</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -5219,77 +4872,68 @@
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="Z1" s="23" t="s">
         <v>72</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="AC1" s="31" t="s">
+      <c r="AC1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="31" t="s">
+      <c r="AD1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF1" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG1" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH1" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="AI1" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ1" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="AK1" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL1" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="AM1" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="AN1" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="AO1" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="AP1" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="AQ1" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="AR1" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS1" s="31" t="s">
+      <c r="AE1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="AT1" s="31" t="s">
+      <c r="AP1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AU1" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="AV1" s="31" t="s">
+      <c r="AQ1" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AR1" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AS1" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -5390,10 +5034,10 @@
         <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2" s="1">
         <v>0</v>
@@ -5407,13 +5051,13 @@
       <c r="AM2" s="1">
         <v>0</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AN2" s="2">
         <v>0</v>
       </c>
       <c r="AO2" s="1">
         <v>0</v>
       </c>
-      <c r="AP2" s="1">
+      <c r="AP2" s="2">
         <v>0</v>
       </c>
       <c r="AQ2" s="1">
@@ -5425,17 +5069,8 @@
       <c r="AS2" s="1">
         <v>0</v>
       </c>
-      <c r="AT2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -5536,52 +5171,43 @@
         <v>0</v>
       </c>
       <c r="AH3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK3" s="1">
+        <v>10</v>
+      </c>
+      <c r="AL3" s="1">
         <v>5</v>
       </c>
-      <c r="AL3" s="1">
-        <v>10</v>
-      </c>
       <c r="AM3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>1</v>
       </c>
       <c r="AO3" s="1">
         <v>1</v>
       </c>
       <c r="AP3" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AQ3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AR3" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>0</v>
       </c>
       <c r="AS3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AU3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -5682,16 +5308,16 @@
         <v>0</v>
       </c>
       <c r="AH4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ4" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK4" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="1">
         <v>0</v>
@@ -5699,14 +5325,14 @@
       <c r="AM4" s="1">
         <v>0</v>
       </c>
-      <c r="AN4" s="1">
-        <v>0</v>
+      <c r="AN4" s="2">
+        <v>2</v>
       </c>
       <c r="AO4" s="1">
         <v>0</v>
       </c>
-      <c r="AP4" s="1">
-        <v>0</v>
+      <c r="AP4" s="2">
+        <v>2</v>
       </c>
       <c r="AQ4" s="1">
         <v>0</v>
@@ -5717,17 +5343,8 @@
       <c r="AS4" s="1">
         <v>0</v>
       </c>
-      <c r="AT4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AU4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -5828,16 +5445,16 @@
         <v>0</v>
       </c>
       <c r="AH5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ5" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK5" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AL5" s="1">
         <v>0</v>
@@ -5845,14 +5462,14 @@
       <c r="AM5" s="1">
         <v>0</v>
       </c>
-      <c r="AN5" s="1">
-        <v>0</v>
+      <c r="AN5" s="2">
+        <v>-1</v>
       </c>
       <c r="AO5" s="1">
         <v>0</v>
       </c>
-      <c r="AP5" s="1">
-        <v>0</v>
+      <c r="AP5" s="2">
+        <v>-1</v>
       </c>
       <c r="AQ5" s="1">
         <v>0</v>
@@ -5863,17 +5480,8 @@
       <c r="AS5" s="1">
         <v>0</v>
       </c>
-      <c r="AT5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AU5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV5" s="2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -5974,10 +5582,10 @@
         <v>0</v>
       </c>
       <c r="AH6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6" s="1">
         <v>0</v>
@@ -5992,34 +5600,25 @@
         <v>0</v>
       </c>
       <c r="AN6" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AO6" s="1">
         <v>0</v>
       </c>
-      <c r="AP6" s="1">
-        <v>0</v>
+      <c r="AP6" s="2">
+        <v>1</v>
       </c>
       <c r="AQ6" s="1">
         <v>0</v>
       </c>
-      <c r="AR6" s="1">
-        <v>10</v>
+      <c r="AR6" s="2">
+        <v>1</v>
       </c>
       <c r="AS6" s="1">
         <v>0</v>
       </c>
-      <c r="AT6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -6120,10 +5719,10 @@
         <v>0</v>
       </c>
       <c r="AH7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ7" s="1">
         <v>0</v>
@@ -6138,13 +5737,13 @@
         <v>0</v>
       </c>
       <c r="AN7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP7" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AQ7" s="1">
         <v>0</v>
@@ -6153,19 +5752,10 @@
         <v>1</v>
       </c>
       <c r="AS7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT7" s="1">
-        <v>10</v>
-      </c>
-      <c r="AU7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -6266,10 +5856,10 @@
         <v>0</v>
       </c>
       <c r="AH8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
@@ -6284,30 +5874,21 @@
         <v>0</v>
       </c>
       <c r="AN8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP8" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ8" s="1">
         <v>0</v>
       </c>
       <c r="AR8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT8" s="1">
-        <v>2</v>
-      </c>
-      <c r="AU8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
give warning for setting k
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/ParameterFile.xlsx
+++ b/doc/Manual/Batchmode/ParameterFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\Desktop\RS3_doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED558CA-9133-425F-96CC-9ECD42827A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E03F5-5AF9-4A6F-9038-115CF90CC598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="117">
   <si>
     <t>Replicates</t>
   </si>
@@ -328,84 +328,6 @@
   </si>
   <si>
     <t>K1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> columns, where </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is the maximum no. of habitats in any one landscape and is set by MaxHabitats in the Control File; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">for LandType = 2 or 9, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> must be 1</t>
-    </r>
   </si>
   <si>
     <t>K2</t>
@@ -637,12 +559,18 @@
   <si>
     <t>Use the same seed for all replicates. 0 = No, 1 = Yes</t>
   </si>
+  <si>
+    <t>n columns, where n is the maximum no. of habitats in any one landscape and is set by MaxHabitats in the Control File; for LandType = 2 or 9, n must be 1</t>
+  </si>
+  <si>
+    <t>K is expressed in individuals/ha, so watch out for discrepancies with cell size and resolution, which are expressed in meters! For example, if cellsize = 1m and K=100, the carrying capacity for a single cell is 100*1^2/10,000=0.01 (functionally zero).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,15 +766,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1074,7 +993,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1217,19 +1136,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1365,7 +1271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1720,23 +1626,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.6640625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="58.5546875" style="22" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="9"/>
+    <col min="1" max="1" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" style="22" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
@@ -1750,7 +1656,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -1761,10 +1667,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1776,7 +1682,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1788,19 +1694,19 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="28"/>
     </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1808,13 +1714,13 @@
         <v>65</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1828,7 +1734,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1842,7 +1748,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1856,7 +1762,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1864,13 +1770,13 @@
         <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1884,7 +1790,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1898,7 +1804,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1912,7 +1818,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -1926,7 +1832,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1934,13 +1840,13 @@
         <v>65</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -1951,10 +1857,10 @@
         <v>64</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1968,7 +1874,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1982,7 +1888,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>14</v>
       </c>
@@ -1996,7 +1902,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>15</v>
       </c>
@@ -2010,7 +1916,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>16</v>
       </c>
@@ -2018,13 +1924,13 @@
         <v>32</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>17</v>
       </c>
@@ -2032,13 +1938,13 @@
         <v>32</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -2049,10 +1955,10 @@
         <v>48</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
@@ -2066,21 +1972,21 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
@@ -2094,9 +2000,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>32</v>
@@ -2108,7 +2014,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>21</v>
       </c>
@@ -2122,7 +2028,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>66</v>
       </c>
@@ -2130,13 +2036,13 @@
         <v>32</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>67</v>
       </c>
@@ -2144,169 +2050,171 @@
         <v>32</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="30"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D31" s="28"/>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="28"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
         <v>83</v>
-      </c>
-      <c r="D32" s="28"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26" t="s">
-        <v>84</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D34" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D35" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="28"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="D36" s="28"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="B37" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C37" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
         <v>93</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
-        <v>94</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="28"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
         <v>95</v>
-      </c>
-      <c r="D38" s="28"/>
-    </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
-        <v>96</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C39" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="28"/>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
         <v>97</v>
-      </c>
-      <c r="D39" s="28"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
-        <v>98</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="27" t="s">
         <v>65</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D42" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>22</v>
       </c>
@@ -2318,7 +2226,7 @@
       </c>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>23</v>
       </c>
@@ -2330,9 +2238,9 @@
       </c>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>65</v>
@@ -2342,7 +2250,7 @@
       </c>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>24</v>
       </c>
@@ -2354,22 +2262,19 @@
       </c>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D47" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D29:D30"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="32767" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2386,53 +2291,53 @@
       <selection pane="bottomRight" activeCell="AU1" sqref="AU1:AU1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.5546875" style="1" customWidth="1"/>
-    <col min="46" max="46" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.109375" style="1"/>
+    <col min="34" max="34" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.5703125" style="1" customWidth="1"/>
+    <col min="46" max="46" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -2443,7 +2348,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -2503,13 +2408,13 @@
         <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
@@ -2518,46 +2423,46 @@
         <v>68</v>
       </c>
       <c r="AC1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="AD1" s="25" t="s">
-        <v>71</v>
-      </c>
       <c r="AE1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="AG1" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO1" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AP1" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AQ1" s="9" t="s">
         <v>22</v>
@@ -2566,16 +2471,16 @@
         <v>23</v>
       </c>
       <c r="AS1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AT1" s="9" t="s">
         <v>24</v>
       </c>
       <c r="AU1" s="23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -2718,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -2861,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -3004,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -3147,7 +3052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -3290,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -3433,7 +3338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -3593,53 +3498,53 @@
       <selection pane="bottomRight" activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.5546875" style="1" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="1"/>
+    <col min="32" max="32" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -3650,7 +3555,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -3710,13 +3615,13 @@
         <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
@@ -3725,40 +3630,40 @@
         <v>68</v>
       </c>
       <c r="AC1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="AE1" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AF1" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AO1" s="9" t="s">
         <v>22</v>
@@ -3767,16 +3672,16 @@
         <v>23</v>
       </c>
       <c r="AQ1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AR1" s="9" t="s">
         <v>24</v>
       </c>
       <c r="AS1" s="23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -3913,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -4050,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -4187,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -4324,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -4461,7 +4366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -4598,7 +4503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -4744,59 +4649,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AS9" sqref="AS9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.5546875" style="1" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="1"/>
+    <col min="32" max="32" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -4807,7 +4712,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -4867,13 +4772,13 @@
         <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
@@ -4882,40 +4787,40 @@
         <v>68</v>
       </c>
       <c r="AC1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="AE1" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AF1" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG1" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AO1" s="9" t="s">
         <v>22</v>
@@ -4924,16 +4829,16 @@
         <v>23</v>
       </c>
       <c r="AQ1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AR1" s="9" t="s">
         <v>24</v>
       </c>
       <c r="AS1" s="23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -5070,7 +4975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -5207,7 +5112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -5344,7 +5249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -5481,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -5618,7 +5523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -5755,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
drop unused map and views features
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/ParameterFile.xlsx
+++ b/doc/Manual/Batchmode/ParameterFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406876A9-5510-4D95-A7EF-6A367F20BFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E578924-8C42-465A-B05D-2DA5CC430E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="375" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="112">
   <si>
     <t>Replicates</t>
   </si>
@@ -171,15 +171,6 @@
     <t>Rmax</t>
   </si>
   <si>
-    <t>SaveMaps</t>
-  </si>
-  <si>
-    <t>MapsInterval</t>
-  </si>
-  <si>
-    <t>DrawLoadedSp</t>
-  </si>
-  <si>
     <t>NOTES</t>
   </si>
   <si>
@@ -193,9 +184,6 @@
   </si>
   <si>
     <t>Competition coefficient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Save maps every  n reproductive seasons </t>
   </si>
   <si>
     <t>FORMAT</t>
@@ -310,9 +298,6 @@
   </si>
   <si>
     <t>Not required for StageStruct = 1</t>
-  </si>
-  <si>
-    <t>Draw loaded species' distribution on the map: 0 = No, 1 = Yes</t>
   </si>
   <si>
     <t>integer</t>
@@ -1713,655 +1698,619 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.6640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="58.5546875" style="17" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="9"/>
+    <col min="1" max="1" width="18.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D5" s="20"/>
     </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C15" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C24" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>32</v>
-      </c>
       <c r="C25" s="28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C29" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="20"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="20"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="20"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="20"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="20"/>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="20"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="20"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="20"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="D39" s="20"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="D44" s="6"/>
-    </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" s="6"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="6"/>
-    </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D47" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2371,64 +2320,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AU8"/>
+  <dimension ref="A1:AR8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU1" sqref="AU1:AU1048576"/>
+      <selection pane="bottomRight" activeCell="AS5" sqref="AS5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.5546875" style="1" customWidth="1"/>
-    <col min="46" max="46" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.109375" style="1"/>
+    <col min="34" max="34" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" style="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2437,7 +2383,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -2470,7 +2416,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>12</v>
@@ -2497,79 +2443,70 @@
         <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="AB1" s="19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="AC1" s="19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="AD1" s="19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AE1" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AF1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AG1" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH1" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="AI1" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AO1" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="AP1" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AQ1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="AS1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AR1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="AT1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AU1" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -2699,20 +2636,11 @@
       <c r="AQ2" s="1">
         <v>0</v>
       </c>
-      <c r="AR2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AR2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -2840,22 +2768,13 @@
         <v>1</v>
       </c>
       <c r="AQ3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -2985,20 +2904,11 @@
       <c r="AQ4" s="1">
         <v>0</v>
       </c>
-      <c r="AR4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AS4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AU4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AR4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -3128,20 +3038,11 @@
       <c r="AQ5" s="1">
         <v>0</v>
       </c>
-      <c r="AR5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AS5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AU5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AR5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -3271,20 +3172,11 @@
       <c r="AQ6" s="1">
         <v>0</v>
       </c>
-      <c r="AR6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AR6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -3412,22 +3304,13 @@
         <v>1</v>
       </c>
       <c r="AQ7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR7" s="1">
-        <v>10</v>
-      </c>
-      <c r="AS7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AU7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -3555,18 +3438,9 @@
         <v>2</v>
       </c>
       <c r="AQ8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR8" s="1">
-        <v>2</v>
-      </c>
-      <c r="AS8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3578,64 +3452,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AS8"/>
+  <dimension ref="A1:AP8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ6" sqref="AQ6"/>
+      <selection pane="bottomRight" activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.5546875" style="1" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="1"/>
+    <col min="32" max="32" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.5703125" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -3644,7 +3515,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -3677,7 +3548,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>12</v>
@@ -3704,73 +3575,64 @@
         <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="AB1" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="AC1" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AD1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF1" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="AG1" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AO1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="AQ1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="AR1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AS1" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -3894,20 +3756,11 @@
       <c r="AO2" s="1">
         <v>0</v>
       </c>
-      <c r="AP2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -4029,22 +3882,13 @@
         <v>1</v>
       </c>
       <c r="AO3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -4168,20 +4012,11 @@
       <c r="AO4" s="1">
         <v>0</v>
       </c>
-      <c r="AP4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AQ4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AS4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -4305,20 +4140,11 @@
       <c r="AO5" s="1">
         <v>0</v>
       </c>
-      <c r="AP5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AQ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AS5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -4442,20 +4268,11 @@
       <c r="AO6" s="1">
         <v>0</v>
       </c>
-      <c r="AP6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -4577,22 +4394,13 @@
         <v>1</v>
       </c>
       <c r="AO7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP7" s="1">
-        <v>10</v>
-      </c>
-      <c r="AQ7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AS7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -4714,18 +4522,9 @@
         <v>2</v>
       </c>
       <c r="AO8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP8" s="1">
-        <v>2</v>
-      </c>
-      <c r="AQ8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4736,63 +4535,60 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AS8"/>
+  <dimension ref="A1:AP8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AS9" sqref="AS9"/>
+      <selection pane="bottomRight" activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.5546875" style="1" customWidth="1"/>
-    <col min="44" max="44" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="1"/>
+    <col min="32" max="32" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.5703125" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -4801,7 +4597,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -4834,7 +4630,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>12</v>
@@ -4861,73 +4657,64 @@
         <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="Z1" s="18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AA1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="AB1" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="AC1" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AD1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF1" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="AG1" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="AH1" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="AI1" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AJ1" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AK1" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AL1" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="AM1" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="AN1" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AO1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="AQ1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="AR1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="AS1" s="18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -5051,20 +4838,11 @@
       <c r="AO2" s="1">
         <v>0</v>
       </c>
-      <c r="AP2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -5186,22 +4964,13 @@
         <v>1</v>
       </c>
       <c r="AO3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -5325,20 +5094,11 @@
       <c r="AO4" s="1">
         <v>0</v>
       </c>
-      <c r="AP4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AQ4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="2">
-        <v>2</v>
-      </c>
-      <c r="AS4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -5462,20 +5222,11 @@
       <c r="AO5" s="1">
         <v>0</v>
       </c>
-      <c r="AP5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AQ5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="AS5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -5599,20 +5350,11 @@
       <c r="AO6" s="1">
         <v>0</v>
       </c>
-      <c r="AP6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -5734,22 +5476,13 @@
         <v>1</v>
       </c>
       <c r="AO7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP7" s="1">
-        <v>10</v>
-      </c>
-      <c r="AQ7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AS7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -5871,18 +5604,9 @@
         <v>2</v>
       </c>
       <c r="AO8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP8" s="1">
-        <v>2</v>
-      </c>
-      <c r="AQ8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
re-write parameterFile changes erased by merge
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/ParameterFile.xlsx
+++ b/doc/Manual/Batchmode/ParameterFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ADCD32-6FD8-446F-81C5-858301B31DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2004CD1B-3A39-43C2-9FAF-4949239FD8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="6525" windowWidth="21600" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <author>Steve Palmer</author>
   </authors>
   <commentList>
-    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="116">
   <si>
     <t>Replicates</t>
   </si>
@@ -571,6 +571,18 @@
   </si>
   <si>
     <t>Seed the RNG of each replicate with its replicate number. 0 = No, 1 = Yes</t>
+  </si>
+  <si>
+    <t>FecSD</t>
+  </si>
+  <si>
+    <t>float &gt; 0</t>
+  </si>
+  <si>
+    <t>Standard deviation of the Normal distribution used to sample the number of offspring.</t>
+  </si>
+  <si>
+    <t>Also used if StageStruct = 1</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1144,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1180,8 +1192,23 @@
     <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="46" applyAlignment="1">
@@ -1256,20 +1283,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="61"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="62">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1 2" xfId="47" xr:uid="{4048FFDC-8701-41F8-8328-E064BBC0A7DC}"/>
     <cellStyle name="20% - Accent2" xfId="22" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2 2" xfId="49" xr:uid="{F971DB0E-3F06-480C-9224-039CCEB11779}"/>
     <cellStyle name="20% - Accent3" xfId="26" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3 2" xfId="51" xr:uid="{51273743-4189-4333-B0C2-B7353B1C0498}"/>
     <cellStyle name="20% - Accent4" xfId="30" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4 2" xfId="53" xr:uid="{7FFD7CED-1465-41D9-BFB2-CFD484867257}"/>
     <cellStyle name="20% - Accent5" xfId="34" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5 2" xfId="55" xr:uid="{22AF6411-26BF-41BE-BC38-A237AC987AC2}"/>
     <cellStyle name="20% - Accent6" xfId="38" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6 2" xfId="57" xr:uid="{5AA5B0D7-8E37-4E76-A0D0-966296E6073B}"/>
     <cellStyle name="40% - Accent1" xfId="19" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1 2" xfId="48" xr:uid="{B58A95CB-1773-40C7-A628-F07CA2E4F9FF}"/>
     <cellStyle name="40% - Accent2" xfId="23" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2 2" xfId="50" xr:uid="{FF81DE82-9FAF-401D-81EC-5915FCDA5F22}"/>
     <cellStyle name="40% - Accent3" xfId="27" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3 2" xfId="52" xr:uid="{2AA581BB-E1EE-4F11-B7F9-542642312D76}"/>
     <cellStyle name="40% - Accent4" xfId="31" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4 2" xfId="54" xr:uid="{A436C8E9-2EDE-4FF4-82C9-53DB6753DE88}"/>
     <cellStyle name="40% - Accent5" xfId="35" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5 2" xfId="56" xr:uid="{A3215F06-0879-4285-A703-5A24FAB16996}"/>
     <cellStyle name="40% - Accent6" xfId="39" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6 2" xfId="58" xr:uid="{211E3D91-CF8D-4D00-89DD-BACD8457200B}"/>
     <cellStyle name="60% - Accent1" xfId="20" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="24" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="28" builtinId="40" customBuiltin="1"/>
@@ -1299,8 +1354,11 @@
     <cellStyle name="Neutral 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 2 2" xfId="59" xr:uid="{D68FD23A-93F9-46B4-BB40-8F999132C465}"/>
     <cellStyle name="Normal 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 3 2" xfId="61" xr:uid="{F21ED733-CE9B-4730-9CC9-7FF814F01752}"/>
     <cellStyle name="Note 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Note 2 2" xfId="60" xr:uid="{9E9A4F82-A6ED-4448-BAFF-5C16428104AE}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="4" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -1606,13 +1664,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2010,81 +2068,81 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>108</v>
+    <row r="29" spans="1:4" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D31" s="23" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="14"/>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32" s="14"/>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>47</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>47</v>
@@ -2092,91 +2150,91 @@
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" s="14"/>
+        <v>82</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>105</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="14"/>
+        <v>86</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D39" s="14"/>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>47</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D40" s="14"/>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>47</v>
@@ -2184,41 +2242,55 @@
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="14"/>
+        <v>96</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C44" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="14"/>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D44" s="14"/>
+      <c r="D45" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2228,13 +2300,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AR8"/>
+  <dimension ref="A1:AS8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ4" sqref="A1:AR8"/>
+      <selection pane="bottomRight" activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2262,25 +2334,26 @@
     <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.5703125" style="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="1"/>
+    <col min="28" max="28" width="5.85546875" style="1" customWidth="1"/>
+    <col min="29" max="30" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5703125" style="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2362,59 +2435,62 @@
       <c r="AA1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AB1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AD1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AE1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AR1" s="24" t="s">
+      <c r="AS1" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -2496,12 +2572,12 @@
       <c r="AA2" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AB2" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AC2" s="1">
         <v>4.5</v>
       </c>
-      <c r="AC2" s="1">
-        <v>0</v>
-      </c>
       <c r="AD2" s="1">
         <v>0</v>
       </c>
@@ -2521,10 +2597,10 @@
         <v>0</v>
       </c>
       <c r="AJ2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL2" s="1">
         <v>0</v>
@@ -2547,8 +2623,11 @@
       <c r="AR2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="AS2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -2630,15 +2709,15 @@
       <c r="AA3" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="AC3" s="1">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AD3" s="1">
         <v>0.98699999999999999</v>
       </c>
-      <c r="AD3" s="1">
-        <v>0</v>
-      </c>
       <c r="AE3" s="1">
         <v>0</v>
       </c>
@@ -2655,34 +2734,37 @@
         <v>0</v>
       </c>
       <c r="AJ3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="1">
         <v>5</v>
       </c>
-      <c r="AM3" s="1">
+      <c r="AN3" s="1">
         <v>10</v>
-      </c>
-      <c r="AN3" s="1">
-        <v>5</v>
       </c>
       <c r="AO3" s="1">
         <v>5</v>
       </c>
       <c r="AP3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AQ3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="AS3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -2764,18 +2846,18 @@
       <c r="AA4" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="30">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1">
         <v>17.7</v>
       </c>
-      <c r="AC4" s="1">
-        <v>0</v>
-      </c>
       <c r="AD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1">
         <v>1.4</v>
       </c>
-      <c r="AE4" s="1">
-        <v>0</v>
-      </c>
       <c r="AF4" s="1">
         <v>0</v>
       </c>
@@ -2789,17 +2871,17 @@
         <v>0</v>
       </c>
       <c r="AJ4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="1">
         <v>5</v>
       </c>
-      <c r="AM4" s="1">
-        <v>0</v>
-      </c>
       <c r="AN4" s="1">
         <v>0</v>
       </c>
@@ -2807,16 +2889,19 @@
         <v>0</v>
       </c>
       <c r="AP4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="1">
         <v>2</v>
       </c>
-      <c r="AQ4" s="1">
-        <v>0</v>
-      </c>
       <c r="AR4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="AS4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -2898,8 +2983,8 @@
       <c r="AA5" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB5" s="1">
-        <v>-9</v>
+      <c r="AB5" s="30">
+        <v>1.8</v>
       </c>
       <c r="AC5" s="1">
         <v>-9</v>
@@ -2908,7 +2993,7 @@
         <v>-9</v>
       </c>
       <c r="AE5" s="1">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="AF5" s="1">
         <v>0</v>
@@ -2923,17 +3008,17 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="1">
         <v>5</v>
       </c>
-      <c r="AM5" s="1">
-        <v>0</v>
-      </c>
       <c r="AN5" s="1">
         <v>0</v>
       </c>
@@ -2941,16 +3026,19 @@
         <v>0</v>
       </c>
       <c r="AP5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="1">
         <v>-1</v>
       </c>
-      <c r="AQ5" s="1">
-        <v>0</v>
-      </c>
       <c r="AR5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="AS5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -3032,12 +3120,12 @@
       <c r="AA6" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="AC6" s="1">
         <v>12</v>
       </c>
-      <c r="AC6" s="1">
-        <v>0</v>
-      </c>
       <c r="AD6" s="1">
         <v>0</v>
       </c>
@@ -3057,13 +3145,13 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="1">
         <v>1</v>
       </c>
       <c r="AL6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM6" s="1">
         <v>0</v>
@@ -3075,16 +3163,19 @@
         <v>0</v>
       </c>
       <c r="AP6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="1">
         <v>10</v>
       </c>
-      <c r="AQ6" s="1">
-        <v>0</v>
-      </c>
       <c r="AR6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="AS6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -3166,8 +3257,8 @@
       <c r="AA7" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB7" s="1">
-        <v>-9</v>
+      <c r="AB7" s="30">
+        <v>3</v>
       </c>
       <c r="AC7" s="1">
         <v>-9</v>
@@ -3176,7 +3267,7 @@
         <v>-9</v>
       </c>
       <c r="AE7" s="1">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="AF7" s="1">
         <v>0</v>
@@ -3191,13 +3282,13 @@
         <v>0</v>
       </c>
       <c r="AJ7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="1">
         <v>1</v>
       </c>
       <c r="AL7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM7" s="1">
         <v>0</v>
@@ -3209,16 +3300,19 @@
         <v>0</v>
       </c>
       <c r="AP7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="AS7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -3300,8 +3394,8 @@
       <c r="AA8" s="1">
         <v>2.5</v>
       </c>
-      <c r="AB8" s="1">
-        <v>-9</v>
+      <c r="AB8" s="30">
+        <v>10</v>
       </c>
       <c r="AC8" s="1">
         <v>-9</v>
@@ -3310,7 +3404,7 @@
         <v>-9</v>
       </c>
       <c r="AE8" s="1">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="AF8" s="1">
         <v>0</v>
@@ -3325,13 +3419,13 @@
         <v>0</v>
       </c>
       <c r="AJ8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="1">
         <v>1</v>
       </c>
       <c r="AL8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM8" s="1">
         <v>0</v>
@@ -3343,12 +3437,15 @@
         <v>0</v>
       </c>
       <c r="AP8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="1">
         <v>2</v>
       </c>
-      <c r="AQ8" s="1">
-        <v>0</v>
-      </c>
       <c r="AR8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3360,13 +3457,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AP8"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK27" sqref="AK26:AK27"/>
+      <selection pane="bottomRight" activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3395,24 +3492,25 @@
     <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.5703125" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="28" max="28" width="5.85546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" style="1" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3494,53 +3592,56 @@
       <c r="AA1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AB1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AP1" s="24" t="s">
+      <c r="AQ1" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -3622,12 +3723,12 @@
       <c r="AA2" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AB2" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AC2" s="1">
         <v>4.5</v>
       </c>
-      <c r="AC2" s="1">
-        <v>0</v>
-      </c>
       <c r="AD2" s="1">
         <v>0</v>
       </c>
@@ -3641,10 +3742,10 @@
         <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ2" s="1">
         <v>0</v>
@@ -3667,8 +3768,11 @@
       <c r="AP2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -3750,12 +3854,12 @@
       <c r="AA3" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="AC3" s="1">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="AC3" s="1">
-        <v>0</v>
-      </c>
       <c r="AD3" s="1">
         <v>0</v>
       </c>
@@ -3769,34 +3873,37 @@
         <v>0</v>
       </c>
       <c r="AH3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="1">
         <v>5</v>
       </c>
-      <c r="AK3" s="1">
+      <c r="AL3" s="1">
         <v>10</v>
-      </c>
-      <c r="AL3" s="1">
-        <v>5</v>
       </c>
       <c r="AM3" s="1">
         <v>5</v>
       </c>
       <c r="AN3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AO3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -3878,12 +3985,12 @@
       <c r="AA4" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="30">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1">
         <v>17.7</v>
       </c>
-      <c r="AC4" s="1">
-        <v>0</v>
-      </c>
       <c r="AD4" s="1">
         <v>0</v>
       </c>
@@ -3897,17 +4004,17 @@
         <v>0</v>
       </c>
       <c r="AH4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="1">
         <v>5</v>
       </c>
-      <c r="AK4" s="1">
-        <v>0</v>
-      </c>
       <c r="AL4" s="1">
         <v>0</v>
       </c>
@@ -3915,16 +4022,19 @@
         <v>0</v>
       </c>
       <c r="AN4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="1">
         <v>2</v>
       </c>
-      <c r="AO4" s="1">
-        <v>0</v>
-      </c>
       <c r="AP4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -4006,12 +4116,12 @@
       <c r="AA5" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="30">
+        <v>1.8</v>
+      </c>
+      <c r="AC5" s="1">
         <v>12</v>
       </c>
-      <c r="AC5" s="1">
-        <v>0</v>
-      </c>
       <c r="AD5" s="1">
         <v>0</v>
       </c>
@@ -4025,17 +4135,17 @@
         <v>0</v>
       </c>
       <c r="AH5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="1">
         <v>5</v>
       </c>
-      <c r="AK5" s="1">
-        <v>0</v>
-      </c>
       <c r="AL5" s="1">
         <v>0</v>
       </c>
@@ -4043,16 +4153,19 @@
         <v>0</v>
       </c>
       <c r="AN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="1">
         <v>-1</v>
       </c>
-      <c r="AO5" s="1">
-        <v>0</v>
-      </c>
       <c r="AP5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -4134,12 +4247,12 @@
       <c r="AA6" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="AC6" s="1">
         <v>12</v>
       </c>
-      <c r="AC6" s="1">
-        <v>0</v>
-      </c>
       <c r="AD6" s="1">
         <v>0</v>
       </c>
@@ -4153,13 +4266,13 @@
         <v>0</v>
       </c>
       <c r="AH6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6" s="1">
         <v>1</v>
       </c>
       <c r="AJ6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="1">
         <v>0</v>
@@ -4171,16 +4284,19 @@
         <v>0</v>
       </c>
       <c r="AN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="1">
         <v>10</v>
       </c>
-      <c r="AO6" s="1">
-        <v>0</v>
-      </c>
       <c r="AP6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -4262,12 +4378,12 @@
       <c r="AA7" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="30">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="1">
         <v>12</v>
       </c>
-      <c r="AC7" s="1">
-        <v>0</v>
-      </c>
       <c r="AD7" s="1">
         <v>0</v>
       </c>
@@ -4281,13 +4397,13 @@
         <v>0</v>
       </c>
       <c r="AH7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="1">
         <v>1</v>
       </c>
       <c r="AJ7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7" s="1">
         <v>0</v>
@@ -4299,16 +4415,19 @@
         <v>0</v>
       </c>
       <c r="AN7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -4390,12 +4509,12 @@
       <c r="AA8" s="1">
         <v>2.5</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AB8" s="30">
+        <v>10</v>
+      </c>
+      <c r="AC8" s="1">
         <v>12</v>
       </c>
-      <c r="AC8" s="1">
-        <v>0</v>
-      </c>
       <c r="AD8" s="1">
         <v>0</v>
       </c>
@@ -4409,13 +4528,13 @@
         <v>0</v>
       </c>
       <c r="AH8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8" s="1">
         <v>1</v>
       </c>
       <c r="AJ8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="1">
         <v>0</v>
@@ -4427,12 +4546,15 @@
         <v>0</v>
       </c>
       <c r="AN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1">
         <v>2</v>
       </c>
-      <c r="AO8" s="1">
-        <v>0</v>
-      </c>
       <c r="AP8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="1">
         <v>0</v>
       </c>
     </row>
@@ -4443,13 +4565,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AP8"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AG3" sqref="AG3"/>
+      <selection pane="bottomRight" activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4477,24 +4599,25 @@
     <col min="25" max="25" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.5703125" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="28" max="28" width="5.85546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5703125" style="1" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -4576,53 +4699,56 @@
       <c r="AA1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AB1" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC1" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AP1" s="24" t="s">
+      <c r="AQ1" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -4704,12 +4830,12 @@
       <c r="AA2" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AB2" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="AC2" s="1">
         <v>4.5</v>
       </c>
-      <c r="AC2" s="1">
-        <v>0</v>
-      </c>
       <c r="AD2" s="1">
         <v>0</v>
       </c>
@@ -4723,10 +4849,10 @@
         <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ2" s="1">
         <v>0</v>
@@ -4749,8 +4875,11 @@
       <c r="AP2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -4832,12 +4961,12 @@
       <c r="AA3" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="AC3" s="1">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="AC3" s="1">
-        <v>0</v>
-      </c>
       <c r="AD3" s="1">
         <v>0</v>
       </c>
@@ -4851,34 +4980,37 @@
         <v>0</v>
       </c>
       <c r="AH3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="1">
         <v>5</v>
       </c>
-      <c r="AK3" s="1">
+      <c r="AL3" s="1">
         <v>10</v>
-      </c>
-      <c r="AL3" s="1">
-        <v>5</v>
       </c>
       <c r="AM3" s="1">
         <v>5</v>
       </c>
       <c r="AN3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AO3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -4960,12 +5092,12 @@
       <c r="AA4" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="30">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1">
         <v>17.7</v>
       </c>
-      <c r="AC4" s="1">
-        <v>0</v>
-      </c>
       <c r="AD4" s="1">
         <v>0</v>
       </c>
@@ -4979,17 +5111,17 @@
         <v>0</v>
       </c>
       <c r="AH4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="1">
         <v>5</v>
       </c>
-      <c r="AK4" s="1">
-        <v>0</v>
-      </c>
       <c r="AL4" s="1">
         <v>0</v>
       </c>
@@ -4997,16 +5129,19 @@
         <v>0</v>
       </c>
       <c r="AN4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="1">
         <v>2</v>
       </c>
-      <c r="AO4" s="1">
-        <v>0</v>
-      </c>
       <c r="AP4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>13</v>
       </c>
@@ -5088,11 +5223,11 @@
       <c r="AA5" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB5" s="1">
-        <v>-9</v>
+      <c r="AB5" s="30">
+        <v>1.8</v>
       </c>
       <c r="AC5" s="1">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="AD5" s="1">
         <v>0</v>
@@ -5107,17 +5242,17 @@
         <v>0</v>
       </c>
       <c r="AH5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="1">
         <v>5</v>
       </c>
-      <c r="AK5" s="1">
-        <v>0</v>
-      </c>
       <c r="AL5" s="1">
         <v>0</v>
       </c>
@@ -5125,16 +5260,19 @@
         <v>0</v>
       </c>
       <c r="AN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="1">
         <v>-1</v>
       </c>
-      <c r="AO5" s="1">
-        <v>0</v>
-      </c>
       <c r="AP5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>14</v>
       </c>
@@ -5216,12 +5354,12 @@
       <c r="AA6" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="AC6" s="1">
         <v>12</v>
       </c>
-      <c r="AC6" s="1">
-        <v>0</v>
-      </c>
       <c r="AD6" s="1">
         <v>0</v>
       </c>
@@ -5235,10 +5373,10 @@
         <v>0</v>
       </c>
       <c r="AH6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6" s="1">
         <v>0</v>
@@ -5253,16 +5391,19 @@
         <v>0</v>
       </c>
       <c r="AN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="1">
         <v>10</v>
       </c>
-      <c r="AO6" s="1">
-        <v>0</v>
-      </c>
       <c r="AP6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -5344,11 +5485,11 @@
       <c r="AA7" s="1">
         <v>1.5</v>
       </c>
-      <c r="AB7" s="1">
-        <v>-9</v>
+      <c r="AB7" s="30">
+        <v>3</v>
       </c>
       <c r="AC7" s="1">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="AD7" s="1">
         <v>0</v>
@@ -5363,10 +5504,10 @@
         <v>0</v>
       </c>
       <c r="AH7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7" s="1">
         <v>0</v>
@@ -5381,16 +5522,19 @@
         <v>0</v>
       </c>
       <c r="AN7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AQ7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -5472,11 +5616,11 @@
       <c r="AA8" s="1">
         <v>2.5</v>
       </c>
-      <c r="AB8" s="1">
-        <v>-9</v>
+      <c r="AB8" s="30">
+        <v>10</v>
       </c>
       <c r="AC8" s="1">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="AD8" s="1">
         <v>0</v>
@@ -5491,10 +5635,10 @@
         <v>0</v>
       </c>
       <c r="AH8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
@@ -5509,12 +5653,15 @@
         <v>0</v>
       </c>
       <c r="AN8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1">
         <v>2</v>
       </c>
-      <c r="AO8" s="1">
-        <v>0</v>
-      </c>
       <c r="AP8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>